<commit_message>
Update - Fixed Camera Profile
Trevor updated the fixed camera profile
</commit_message>
<xml_diff>
--- a/Fixed Camera-Element_Profile.xlsx
+++ b/Fixed Camera-Element_Profile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paululisse/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorbernhard/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E81555-B4A8-554B-9B58-D5B894BCD443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9837D6-F7C3-4F45-B01B-5CCF0012B0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Element Profiles" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5748" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5769" uniqueCount="370">
   <si>
     <t>Export date: Nov 04, 2024</t>
   </si>
@@ -1034,9 +1034,6 @@
     <t>Corner Bracket - R100/R120/R200/R360/R400</t>
   </si>
   <si>
-    <t>ACC-R2-CAP</t>
-  </si>
-  <si>
     <t>Accessory26</t>
   </si>
   <si>
@@ -1119,6 +1116,33 @@
   </si>
   <si>
     <t>ACC-R3-JBW</t>
+  </si>
+  <si>
+    <t>Accessory31</t>
+  </si>
+  <si>
+    <t>R520 Junction Box</t>
+  </si>
+  <si>
+    <t>ACC-R52-JB</t>
+  </si>
+  <si>
+    <t>Accessory32</t>
+  </si>
+  <si>
+    <t>Accessory33</t>
+  </si>
+  <si>
+    <t>DR40 Wall Plate</t>
+  </si>
+  <si>
+    <t>ACC-DR40-WP</t>
+  </si>
+  <si>
+    <t>ACC-DR40-AWM</t>
+  </si>
+  <si>
+    <t>DR40 Angle Wall Mount</t>
   </si>
 </sst>
 </file>
@@ -1648,8 +1672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:SJ128"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="G120" sqref="G120"/>
+    <sheetView tabSelected="1" topLeftCell="B95" workbookViewId="0">
+      <selection activeCell="R124" sqref="R124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2755,16 +2779,16 @@
         <v>27</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AC3" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="AD3" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="AD3" s="3" t="s">
-        <v>351</v>
-      </c>
       <c r="AE3" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AF3" s="3"/>
       <c r="AG3" s="3"/>
@@ -3314,19 +3338,19 @@
         <v>30</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AB4" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AC4" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="AD4" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="AD4" s="5" t="s">
-        <v>351</v>
-      </c>
       <c r="AE4" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AF4" s="5"/>
       <c r="AG4" s="5"/>
@@ -5889,16 +5913,16 @@
         <v>43</v>
       </c>
       <c r="AB7" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AD7" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AE7" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AF7" s="5"/>
       <c r="AG7" s="5"/>
@@ -7006,19 +7030,19 @@
         <v>68</v>
       </c>
       <c r="AA9" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AB9" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="AD9" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="AC9" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="AD9" s="5" t="s">
+      <c r="AE9" s="5" t="s">
         <v>354</v>
-      </c>
-      <c r="AE9" s="5" t="s">
-        <v>355</v>
       </c>
       <c r="AF9" s="5"/>
       <c r="AG9" s="5"/>
@@ -38707,16 +38731,16 @@
         <v>157</v>
       </c>
       <c r="AB58" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AC58" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AD58" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AE58" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AF58" s="5"/>
       <c r="AG58" s="5"/>
@@ -70819,16 +70843,16 @@
         <v>239</v>
       </c>
       <c r="AB116" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AC116" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AD116" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AE116" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AF116" s="10"/>
       <c r="AG116" s="10"/>
@@ -72356,9 +72380,15 @@
       <c r="O119" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="P119" s="10"/>
-      <c r="Q119" s="10"/>
-      <c r="R119" s="10"/>
+      <c r="P119" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q119" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="R119" s="10" t="s">
+        <v>244</v>
+      </c>
       <c r="S119" s="10" t="s">
         <v>244</v>
       </c>
@@ -72899,10 +72929,18 @@
       <c r="N120" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="O120" s="10"/>
-      <c r="P120" s="10"/>
-      <c r="Q120" s="10"/>
-      <c r="R120" s="10"/>
+      <c r="O120" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="P120" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q120" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="R120" s="10" t="s">
+        <v>246</v>
+      </c>
       <c r="S120" s="10"/>
       <c r="T120" s="10"/>
       <c r="U120" s="10"/>
@@ -72916,19 +72954,23 @@
       <c r="Y120" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="Z120" s="10"/>
-      <c r="AA120" s="10"/>
+      <c r="Z120" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="AA120" s="10" t="s">
+        <v>366</v>
+      </c>
       <c r="AB120" s="10" t="s">
-        <v>247</v>
+        <v>362</v>
       </c>
       <c r="AC120" s="10" t="s">
-        <v>247</v>
+        <v>362</v>
       </c>
       <c r="AD120" s="10" t="s">
-        <v>247</v>
+        <v>362</v>
       </c>
       <c r="AE120" s="10" t="s">
-        <v>247</v>
+        <v>362</v>
       </c>
       <c r="AF120" s="10"/>
       <c r="AG120" s="10"/>
@@ -77565,10 +77607,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -78092,7 +78134,7 @@
         <v>45</v>
       </c>
       <c r="D26" t="s">
-        <v>333</v>
+        <v>302</v>
       </c>
       <c r="E26">
         <v>49</v>
@@ -78103,16 +78145,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>333</v>
+      </c>
+      <c r="B27" t="s">
         <v>334</v>
-      </c>
-      <c r="B27" t="s">
-        <v>335</v>
       </c>
       <c r="C27" t="s">
         <v>45</v>
       </c>
       <c r="D27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E27">
         <v>79</v>
@@ -78123,16 +78165,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>336</v>
+      </c>
+      <c r="B28" t="s">
         <v>337</v>
-      </c>
-      <c r="B28" t="s">
-        <v>338</v>
       </c>
       <c r="C28" t="s">
         <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E28">
         <v>49</v>
@@ -78143,16 +78185,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>339</v>
+      </c>
+      <c r="B29" t="s">
         <v>340</v>
-      </c>
-      <c r="B29" t="s">
-        <v>341</v>
       </c>
       <c r="C29" t="s">
         <v>45</v>
       </c>
       <c r="D29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E29">
         <v>49</v>
@@ -78163,16 +78205,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>342</v>
+      </c>
+      <c r="B30" t="s">
         <v>343</v>
-      </c>
-      <c r="B30" t="s">
-        <v>344</v>
       </c>
       <c r="C30" t="s">
         <v>45</v>
       </c>
       <c r="D30" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E30">
         <v>49</v>
@@ -78183,21 +78225,81 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>358</v>
+      </c>
+      <c r="B31" t="s">
         <v>359</v>
-      </c>
-      <c r="B31" t="s">
-        <v>360</v>
       </c>
       <c r="C31" t="s">
         <v>45</v>
       </c>
       <c r="D31" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E31">
         <v>69</v>
       </c>
       <c r="F31">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>361</v>
+      </c>
+      <c r="B32" t="s">
+        <v>362</v>
+      </c>
+      <c r="C32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" t="s">
+        <v>363</v>
+      </c>
+      <c r="E32">
+        <v>79</v>
+      </c>
+      <c r="F32">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>364</v>
+      </c>
+      <c r="B33" t="s">
+        <v>366</v>
+      </c>
+      <c r="C33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" t="s">
+        <v>367</v>
+      </c>
+      <c r="E33">
+        <v>25</v>
+      </c>
+      <c r="F33">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>365</v>
+      </c>
+      <c r="B34" t="s">
+        <v>369</v>
+      </c>
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" t="s">
+        <v>368</v>
+      </c>
+      <c r="E34">
+        <v>25</v>
+      </c>
+      <c r="F34">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>